<commit_message>
Add Procfile for Render deployment
</commit_message>
<xml_diff>
--- a/coupons.xlsx
+++ b/coupons.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -497,15 +497,33 @@
           <t>rushika</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>123456789</t>
-        </is>
+      <c r="B4" t="n">
+        <v>123456789</v>
       </c>
       <c r="C4" t="n">
         <v>5</v>
       </c>
       <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-08-16</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Venkateswarrao V</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>99999</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>14</v>
+      </c>
+      <c r="D5" t="inlineStr">
         <is>
           <t>2025-08-16</t>
         </is>

</xml_diff>